<commit_message>
[feat] Player, Flashlight, StatusEffect 데이터 추가
</commit_message>
<xml_diff>
--- a/Monster.xlsx
+++ b/Monster.xlsx
@@ -410,7 +410,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -419,8 +419,9 @@
     <col min="4" max="4" width="24.625" customWidth="1"/>
     <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="14.75" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="7" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="19.125" customWidth="1"/>
+    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[feat] Monster, Skill data 수정
</commit_message>
<xml_diff>
--- a/Monster.xlsx
+++ b/Monster.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,47 +41,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>일반 적 타입의 보스 신체 일부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nomal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{Skill_Boss_Dash}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GrabGage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스타입의 적 본체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enemy_Boss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Enemy_Mob_A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>일반 적 타입의 보스 신체 일부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nomal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{Skill_Boss_Dash}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GrabGage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>보스타입의 적 본체</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enemy_Boss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DataId</t>
+    <t>SkillDistance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -419,23 +423,22 @@
     <col min="4" max="4" width="24.625" customWidth="1"/>
     <col min="5" max="5" width="10.125" customWidth="1"/>
     <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="17.125" customWidth="1"/>
-    <col min="8" max="8" width="19.125" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.75" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -447,47 +450,53 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
+      <c r="J1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>0.7</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2">
+        <v>130</v>
+      </c>
+      <c r="I2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -495,7 +504,7 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feat] Player flashlight 데이터 수정
</commit_message>
<xml_diff>
--- a/Monster.xlsx
+++ b/Monster.xlsx
@@ -89,7 +89,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DeadEndDistane</t>
+    <t>DeadEndDistance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -418,7 +418,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>